<commit_message>
add testcase val check
</commit_message>
<xml_diff>
--- a/WebTest/WebTest/TestCase/TestCaseTemplate.xlsx
+++ b/WebTest/WebTest/TestCase/TestCaseTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB837F56-5156-449A-ABFC-3E79434D4601}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8E1F52-ABA9-4F01-8B48-C355936BAF65}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="120">
   <si>
     <t>TextBox</t>
   </si>
@@ -404,6 +404,19 @@
   </si>
   <si>
     <t>C:/ExampleHTML/WebTestExample1.html</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>実行ボタン押下種別（0:Submit 1:Click）</t>
+    <rPh sb="0" eb="2">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>オウカ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>シュベツ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -603,6 +616,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -622,12 +641,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -971,7 +984,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -985,58 +998,58 @@
         <v>23</v>
       </c>
       <c r="B1" s="16"/>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="16"/>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
     </row>
     <row r="3" spans="1:14" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
@@ -1081,10 +1094,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="12" t="s">
         <v>4</v>
       </c>
@@ -1123,10 +1136,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="14" t="s">
         <v>22</v>
       </c>
@@ -1165,10 +1178,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="25"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="3">
         <v>1</v>
       </c>
@@ -1207,10 +1220,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="25"/>
+      <c r="A8" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="17"/>
       <c r="C8" s="3">
         <v>0</v>
       </c>
@@ -2298,17 +2311,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:N1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:N2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:N3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2335,54 +2348,54 @@
         <v>23</v>
       </c>
       <c r="B1" s="16"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="16"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
     </row>
     <row r="3" spans="1:14" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
@@ -2427,10 +2440,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2445,10 +2458,10 @@
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="14"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -2463,10 +2476,10 @@
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="25"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -2481,10 +2494,10 @@
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -2904,17 +2917,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:N1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:N2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:N3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>